<commit_message>
troubleshooting colinearitty issues, update brain region list
</commit_message>
<xml_diff>
--- a/prep/brain_measures_descriptions.xlsx
+++ b/prep/brain_measures_descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GenScotDepression/users/niamh/puberty_ABCD/ABCD_puberty_depression/prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534A5FE9-1112-7847-8E58-F349F8D308B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A396672-BAEE-5942-B4C4-11F640BDC350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="-21100" windowWidth="27260" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6040" yWindow="-25460" windowWidth="37820" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ls.DTI_region_replacement_label" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>Field name/Abbreviation</t>
   </si>
@@ -303,109 +303,127 @@
     <t>Subcortical grey volume</t>
   </si>
   <si>
-    <t xml:space="preserve">fx	</t>
-  </si>
-  <si>
-    <t>Fornix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cc	</t>
-  </si>
-  <si>
-    <t>Corpus Callosum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fmaj	</t>
-  </si>
-  <si>
-    <t>Foreceps Major</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fmin	</t>
-  </si>
-  <si>
-    <t>Foreceps Minor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atr	</t>
-  </si>
-  <si>
-    <t>Anterior Thalamic Radiations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cgc	</t>
-  </si>
-  <si>
-    <t>Cingulate Cingulum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cgh	</t>
-  </si>
-  <si>
-    <t>Parahippocampal Cingulum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cst	</t>
-  </si>
-  <si>
-    <t>Corticospinal/Pyramidal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifo	</t>
-  </si>
-  <si>
-    <t>Inferior-Fronto-Occipital Fasiculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ifsfc	</t>
-  </si>
-  <si>
-    <t>Inferior Frontal Superior Frontal Cortex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ilf	</t>
-  </si>
-  <si>
-    <t>Inferior Longitudinal Fasiculus</t>
-  </si>
-  <si>
-    <t>Parietal Superior Longitudinal Fasiculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scs	</t>
-  </si>
-  <si>
-    <t>Superior Corticostriate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sifc	</t>
-  </si>
-  <si>
-    <t>Striatal Inferior Frontal Cortex</t>
-  </si>
-  <si>
-    <t>Superior Longitudinal Fasiculus</t>
-  </si>
-  <si>
-    <t>Temporal Superior Longitudinal Fasiculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unc	</t>
-  </si>
-  <si>
-    <t>Uncinate Fasciculus</t>
-  </si>
-  <si>
     <t>dMRI tracts</t>
   </si>
   <si>
-    <t xml:space="preserve">tslf	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slf	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pslf	</t>
+    <t>fornix</t>
+  </si>
+  <si>
+    <t>cingulate cingulum</t>
+  </si>
+  <si>
+    <t>parahippocampal cingulum</t>
+  </si>
+  <si>
+    <t>anterior thalamic radiations</t>
+  </si>
+  <si>
+    <t>uncinate</t>
+  </si>
+  <si>
+    <t>inferior longitudinal fasciculus</t>
+  </si>
+  <si>
+    <t>inferior frontal occipital fasciculus</t>
+  </si>
+  <si>
+    <t>forceps major</t>
+  </si>
+  <si>
+    <t>forceps minor</t>
+  </si>
+  <si>
+    <t>corpus callosum</t>
+  </si>
+  <si>
+    <t>superior longitudinal fasciculus</t>
+  </si>
+  <si>
+    <t>temporal superior longitudinal fasciculus (arcuate fasciculus)</t>
+  </si>
+  <si>
+    <t>parietal superior longitudinal fasciculus</t>
+  </si>
+  <si>
+    <t>superior corticostriate</t>
+  </si>
+  <si>
+    <t>frontal superior corticostriate</t>
+  </si>
+  <si>
+    <t>parietal superior corticostriate</t>
+  </si>
+  <si>
+    <t>striatal inferior frontal cortex tract</t>
+  </si>
+  <si>
+    <t>inferior frontal to superior frontal cortical tract</t>
+  </si>
+  <si>
+    <t>corticospinal tract (pyramidal tract)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fornix excluding fimbria </t>
+  </si>
+  <si>
+    <t>fx</t>
+  </si>
+  <si>
+    <t>fxcut</t>
+  </si>
+  <si>
+    <t>cgc</t>
+  </si>
+  <si>
+    <t>cgh</t>
+  </si>
+  <si>
+    <t>cst</t>
+  </si>
+  <si>
+    <t>atr</t>
+  </si>
+  <si>
+    <t>unc</t>
+  </si>
+  <si>
+    <t>ilf</t>
+  </si>
+  <si>
+    <t>ifo</t>
+  </si>
+  <si>
+    <t>fmaj</t>
+  </si>
+  <si>
+    <t>fmin</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>slf</t>
+  </si>
+  <si>
+    <t>tslf</t>
+  </si>
+  <si>
+    <t>pslf</t>
+  </si>
+  <si>
+    <t>scs</t>
+  </si>
+  <si>
+    <t>fscs</t>
+  </si>
+  <si>
+    <t>pscs</t>
+  </si>
+  <si>
+    <t>sifc</t>
+  </si>
+  <si>
+    <t>ifsfc</t>
   </si>
 </sst>
 </file>
@@ -782,7 +800,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -915,6 +933,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -960,7 +987,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -983,8 +1010,15 @@
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1340,16 +1374,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.1640625" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
     <col min="3" max="3" width="32.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" customWidth="1"/>
@@ -1762,146 +1796,170 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="B47" s="12"/>
     </row>
     <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
-        <v>90</v>
+      <c r="A48" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="B48" s="12" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="12" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="12" t="s">
+    </row>
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="s">
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="12" t="s">
+    </row>
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="12" t="s">
+    </row>
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="13" t="s">
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="12" t="s">
+    </row>
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B60" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="13" t="s">
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B61" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B54" s="12" t="s">
+    </row>
+    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B62" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="13" t="s">
+    <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="12" t="s">
+    </row>
+    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="13" t="s">
+    <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="12" t="s">
+    </row>
+    <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="13" t="s">
+    <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" s="12" t="s">
         <v>108</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1911,9 +1969,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2140,19 +2201,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07CD3CC-01CA-48E6-A305-68AA52F811F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77232F5D-4BD7-4169-AB35-5CC6570F243F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2177,9 +2234,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77232F5D-4BD7-4169-AB35-5CC6570F243F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D07CD3CC-01CA-48E6-A305-68AA52F811F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>